<commit_message>
Edit Detail Design about practise plan
</commit_message>
<xml_diff>
--- a/Fit/Docs/DB Design.xlsx
+++ b/Fit/Docs/DB Design.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="98">
   <si>
     <t>TFit_AdminUsers</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -298,6 +298,114 @@
   </si>
   <si>
     <t>LowerLeg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>can not edit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Weight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ActionId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TFit_Events</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Groups</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Count</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Count of each group</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TFit_Plan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EventId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TFit_EventGroups</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EventSeq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GroupSeq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EventGroupId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DaysAfterPrev</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bigint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bigint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TFit_Schedule</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Year</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Month</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsFinished</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -654,17 +762,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B111"/>
+  <dimension ref="A1:C149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A111" sqref="A111"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="B141" sqref="B141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="27.375" customWidth="1"/>
     <col min="2" max="2" width="17.25" customWidth="1"/>
-    <col min="3" max="3" width="10.25" customWidth="1"/>
+    <col min="3" max="3" width="36.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
@@ -974,12 +1082,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>1</v>
       </c>
@@ -987,7 +1095,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
         <v>3</v>
       </c>
@@ -995,7 +1103,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
         <v>41</v>
       </c>
@@ -1003,7 +1111,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
         <v>17</v>
       </c>
@@ -1011,7 +1119,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -1019,12 +1127,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C56" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
         <v>1</v>
       </c>
@@ -1032,7 +1143,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
         <v>3</v>
       </c>
@@ -1040,7 +1151,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
         <v>17</v>
       </c>
@@ -1048,7 +1159,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
         <v>19</v>
       </c>
@@ -1056,12 +1167,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C62" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
         <v>1</v>
       </c>
@@ -1069,7 +1183,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
         <v>3</v>
       </c>
@@ -1331,10 +1445,10 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A102" t="s">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="B102" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.15">
@@ -1386,6 +1500,266 @@
     <row r="111" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A111" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A112" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A114" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A115" t="s">
+        <v>1</v>
+      </c>
+      <c r="B115" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A116" t="s">
+        <v>17</v>
+      </c>
+      <c r="B116" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A117" t="s">
+        <v>19</v>
+      </c>
+      <c r="B117" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A118" t="s">
+        <v>75</v>
+      </c>
+      <c r="B118" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A119" t="s">
+        <v>74</v>
+      </c>
+      <c r="B119" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A120" t="s">
+        <v>77</v>
+      </c>
+      <c r="B120" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A121" t="s">
+        <v>78</v>
+      </c>
+      <c r="B121" t="s">
+        <v>87</v>
+      </c>
+      <c r="C121" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A123" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A124" t="s">
+        <v>1</v>
+      </c>
+      <c r="B124" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A125" t="s">
+        <v>17</v>
+      </c>
+      <c r="B125" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A126" t="s">
+        <v>19</v>
+      </c>
+      <c r="B126" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A127" t="s">
+        <v>82</v>
+      </c>
+      <c r="B127" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A128" t="s">
+        <v>81</v>
+      </c>
+      <c r="B128" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A129" t="s">
+        <v>84</v>
+      </c>
+      <c r="B129" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A130" t="s">
+        <v>85</v>
+      </c>
+      <c r="B130" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A132" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A133" t="s">
+        <v>1</v>
+      </c>
+      <c r="B133" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A134" t="s">
+        <v>17</v>
+      </c>
+      <c r="B134" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A135" t="s">
+        <v>19</v>
+      </c>
+      <c r="B135" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A136" t="s">
+        <v>90</v>
+      </c>
+      <c r="B136" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A137" t="s">
+        <v>86</v>
+      </c>
+      <c r="B137" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A138" t="s">
+        <v>88</v>
+      </c>
+      <c r="B138" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A140" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A141" t="s">
+        <v>1</v>
+      </c>
+      <c r="B141" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A142" t="s">
+        <v>17</v>
+      </c>
+      <c r="B142" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A143" t="s">
+        <v>19</v>
+      </c>
+      <c r="B143" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A144" t="s">
+        <v>93</v>
+      </c>
+      <c r="B144" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A145" t="s">
+        <v>86</v>
+      </c>
+      <c r="B145" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A146" t="s">
+        <v>94</v>
+      </c>
+      <c r="B146" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A147" t="s">
+        <v>95</v>
+      </c>
+      <c r="B147" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A148" t="s">
+        <v>96</v>
+      </c>
+      <c r="B148" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A149" t="s">
+        <v>97</v>
+      </c>
+      <c r="B149" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1399,7 +1773,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>

</xml_diff>

<commit_message>
AdminLog Completed, FrontWeb User some
</commit_message>
<xml_diff>
--- a/Fit/Docs/DB Design.xlsx
+++ b/Fit/Docs/DB Design.xlsx
@@ -258,54 +258,163 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Age</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gender</t>
+    <t>LowerArm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Waist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UpperLeg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LowerLeg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>can not edit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Weight</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TFit_Schedule</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Year</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Month</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsFinished</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountUnit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nvarchar(50)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TFit_ActionPackages</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bigint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PackageSeq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>LowerArm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Chest</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Waist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hip</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UpperLeg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LowerLeg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>can not edit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UserId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Weight</t>
+    <t>DaysFromPrev</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TFit_ActionsInPkg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">PackageId </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ActionId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GroupCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MoveCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intensity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>decimal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PackageId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>计划安排</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RBAC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>操作日志</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>枚举项</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前台用户</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>围度记录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TFit_RolePermissions</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -313,123 +422,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TFit_Schedule</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UserId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Year</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Month</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Day</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IsFinished</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CountUnit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nvarchar(50)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TFit_ActionPackages</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UserId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bigint</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PackageSeq</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DaysFromPrev</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TFit_ActionsInPkg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">PackageId </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ActionId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GroupCount</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MoveCount</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Intensity</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>decimal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PackageId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>计划安排</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RBAC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>操作日志</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>枚举项</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>设置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>前台用户</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>围度记录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TFit_RolePermissions</t>
+    <t>IsActivated</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OperateCode</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -815,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C149"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -828,7 +829,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -1000,7 +1001,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
@@ -1042,7 +1043,7 @@
     </row>
     <row r="35" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A35" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
@@ -1100,7 +1101,7 @@
     </row>
     <row r="44" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A44" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
@@ -1150,7 +1151,7 @@
     </row>
     <row r="52" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A52" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.15">
@@ -1200,7 +1201,7 @@
     </row>
     <row r="60" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A60" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.15">
@@ -1226,63 +1227,63 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="B64" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="B65" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B66" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B67" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B68" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B69" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A70" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B70" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B71" t="s">
         <v>16</v>
@@ -1290,23 +1291,23 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
-        <v>17</v>
+        <v>103</v>
       </c>
       <c r="B72" t="s">
-        <v>18</v>
+        <v>100</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
-        <v>19</v>
+        <v>101</v>
       </c>
       <c r="B73" t="s">
-        <v>16</v>
+        <v>102</v>
       </c>
     </row>
     <row r="75" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A75" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.15">
@@ -1324,7 +1325,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B78" t="s">
         <v>2</v>
@@ -1353,42 +1354,42 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="90" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A90" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.15">
@@ -1396,7 +1397,7 @@
         <v>42</v>
       </c>
       <c r="C91" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.15">
@@ -1436,7 +1437,7 @@
         <v>45</v>
       </c>
       <c r="C97" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.15">
@@ -1542,10 +1543,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A112" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B112" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.15">
@@ -1603,7 +1604,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A122" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.15">
@@ -1632,31 +1633,31 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A126" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B126" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A127" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B127" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A128" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B128" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A130" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.15">
@@ -1685,47 +1686,47 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A134" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B134" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A135" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B135" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A136" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B136" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A137" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B137" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A138" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B138" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A140" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.15">
@@ -1754,7 +1755,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A144" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B144" t="s">
         <v>2</v>
@@ -1762,7 +1763,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A145" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B145" t="s">
         <v>2</v>
@@ -1770,31 +1771,31 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A146" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B146" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A147" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B147" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A148" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B148" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A149" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B149" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
FrontWeb login, AdminWeb UserInfo
</commit_message>
<xml_diff>
--- a/Fit/Docs/DB Design.xlsx
+++ b/Fit/Docs/DB Design.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="103">
   <si>
     <t>TFit_AdminUsers</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -415,10 +415,6 @@
   </si>
   <si>
     <t>TFit_RolePermissions</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -816,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1291,18 +1287,18 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B72" t="s">
-        <v>100</v>
+        <v>6</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
+        <v>100</v>
+      </c>
+      <c r="B73" t="s">
         <v>101</v>
-      </c>
-      <c r="B73" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="75" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.15">

</xml_diff>